<commit_message>
Entidad Relacion - Plataformas
</commit_message>
<xml_diff>
--- a/database/seeders/AsignarAlias.xlsx
+++ b/database/seeders/AsignarAlias.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$6351</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$6719</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19053" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20137" uniqueCount="127">
   <si>
     <t>Spoon - Mall San Pedro</t>
   </si>
@@ -358,6 +358,57 @@
   <si>
     <t>Spoon - Oxígeno</t>
   </si>
+  <si>
+    <t>PEYA</t>
+  </si>
+  <si>
+    <t>Spoon Plaza La Trinidad</t>
+  </si>
+  <si>
+    <t>Spoon Yoses</t>
+  </si>
+  <si>
+    <t>Spoon San Francisco De Heredia</t>
+  </si>
+  <si>
+    <t>Spoon Sabana</t>
+  </si>
+  <si>
+    <t>Spoon Real Cariari 257</t>
+  </si>
+  <si>
+    <t>Spoon Distrito 4</t>
+  </si>
+  <si>
+    <t>Spoon Paseo De Las Flores</t>
+  </si>
+  <si>
+    <t>Spoon Plaza Heredia</t>
+  </si>
+  <si>
+    <t>Spoon Escazu Village</t>
+  </si>
+  <si>
+    <t>Spoon Sabanilla</t>
+  </si>
+  <si>
+    <t>Spoon Ciudad Del Este</t>
+  </si>
+  <si>
+    <t>Spoon Pinares</t>
+  </si>
+  <si>
+    <t>Spoon Plaza De La Cultura</t>
+  </si>
+  <si>
+    <t>Spoon Plaza Real</t>
+  </si>
+  <si>
+    <t>Spoon Clínica Bíblica</t>
+  </si>
+  <si>
+    <t>Spoon Plaza Del Sol</t>
+  </si>
 </sst>
 </file>
 
@@ -398,10 +449,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,16 +737,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6352"/>
+  <dimension ref="A1:C6719"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1088" sqref="H1088"/>
+      <pane ySplit="1" topLeftCell="A6578" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6585" sqref="C6585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -70557,10 +70613,3995 @@
       </c>
     </row>
     <row r="6352" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6352" s="1"/>
+      <c r="A6352" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6352" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6352" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6353" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6353" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6353" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6354" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6354" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6354" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6355" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6355" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6355" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6356" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6356" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6356" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6357" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6357" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6357" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6358" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6358" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6358" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6359" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6359" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6359" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6360" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6360" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6360" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6361" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6361" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6361" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6362" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6362" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6362" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6363" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6363" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6363" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6364" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6364" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6364" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6365" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6365" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6365" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6366" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6366" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6366" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6367" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6367" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6367" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6368" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6368" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6368" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6369" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6369" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6369" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6370" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6370" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6370" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6371" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6371" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6371" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6372" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6372" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6372" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6373" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6373" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6373" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6374" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6374" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6374" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6375" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6375" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6375" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6376" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6376" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6377" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6377" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6377" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6378" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6378" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6378" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6379" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6379" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6379" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6380" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6380" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6380" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6381" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6381" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6381" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6382" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6382" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6382" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6383" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6383" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6383" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6384" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6384" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6384" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6385" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6385" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6385" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6386" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6386" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6387" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6387" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6387" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6388" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6388" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6388" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6389" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6389" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6389" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6390" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6390" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6390" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6391" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6391" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6391" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6392" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6392" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6392" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6393" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6393" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6393" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6394" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6394" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6394" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6395" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6395" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6395" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6396" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6396" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6396" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6397" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6397" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6397" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6398" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6398" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6398" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6399" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6399" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6399" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6400" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6400" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6400" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6401" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6401" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6401" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6402" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6402" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6402" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6403" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6403" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6404" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6404" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6404" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6405" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6405" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6405" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6406" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6406" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6406" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6407" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6407" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6407" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6408" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6408" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6408" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6409" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6409" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6410" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6410" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6410" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6411" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6411" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6411" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6412" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6412" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6413" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6413" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6413" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6414" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6414" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6414" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6415" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6415" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6416" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6416" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6416" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6417" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6417" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6418" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6418" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6418" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6419" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6419" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6419" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6420" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6420" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6420" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6421" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6421" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6421" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6422" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6422" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6422" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6423" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6423" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6423" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6424" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6424" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6424" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6425" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6425" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6425" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6426" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6426" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6426" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6427" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6427" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6427" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6428" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6428" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6428" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6429" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6429" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6429" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6429" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6430" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6430" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6430" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6430" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6431" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6431" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6431" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6432" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6432" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6432" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6433" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6433" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6433" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6433" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6434" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6434" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6434" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6435" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6435" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6435" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6436" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6436" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6436" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6437" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6437" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6437" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6438" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6438" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6438" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6439" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6439" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6439" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6440" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6440" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6440" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6441" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6441" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6441" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6441" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6442" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6442" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6442" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6443" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6443" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6443" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6444" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6444" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6444" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6444" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6445" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6445" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6445" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6445" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6446" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6446" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6446" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6447" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6447" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6447" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6447" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6448" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6448" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6448" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6448" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6449" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6449" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6449" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6450" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6450" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6450" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6451" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6451" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6451" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6451" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6452" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6452" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6452" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6453" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6453" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6453" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6454" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6454" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6454" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6455" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6455" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6455" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6456" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6456" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6456" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6457" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6457" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6457" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6458" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6458" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6458" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6459" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6459" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6459" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6460" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6460" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6460" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6461" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6461" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6461" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6462" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6462" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6462" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6463" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6463" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6463" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6464" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6464" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6464" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6465" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6465" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6465" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6466" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6466" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6466" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6467" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6467" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6467" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6468" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6468" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6469" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6469" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6469" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6470" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6470" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6470" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6471" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6471" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6471" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6472" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6472" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6472" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6473" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6473" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6473" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6474" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6474" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6474" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6475" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6475" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6475" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6476" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6476" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6476" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6477" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6477" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6477" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6478" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6478" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6478" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6479" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6479" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6479" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6480" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6480" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6480" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6481" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6481" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6481" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6482" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6482" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6482" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6483" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6483" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6483" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6484" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6484" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6484" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6485" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6485" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6485" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6486" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6486" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6486" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6487" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6487" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6488" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6488" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6488" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6489" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6489" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6489" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6490" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6490" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6490" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6491" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6491" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6491" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6492" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6492" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6492" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6493" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6493" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6493" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6494" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6494" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6494" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6495" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6495" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6495" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6496" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6496" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6496" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6497" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6497" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6497" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6498" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6498" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6498" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6499" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6499" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6499" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6500" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6500" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6500" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6501" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6501" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6501" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6502" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6502" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6502" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6502" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6503" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6503" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6503" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6504" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6504" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6504" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6505" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6505" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6505" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6506" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6506" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6506" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6507" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6507" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6507" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6508" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6508" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6508" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6509" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6509" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6509" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6510" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6510" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6510" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6511" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6511" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6512" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6512" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6512" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6513" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6513" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6513" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6514" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6514" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6514" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6515" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6515" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6515" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6516" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6516" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6516" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6517" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6517" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6517" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6518" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6518" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6518" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6519" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6519" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6519" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6520" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6520" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6520" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6521" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6521" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6521" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6522" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6522" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6522" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6523" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6523" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6523" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6524" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6524" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6524" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6525" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6525" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6525" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6525" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6526" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6526" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6526" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6526" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6527" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6527" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6527" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6528" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6528" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6528" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6528" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6529" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6529" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6529" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6529" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6530" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6530" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6530" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6530" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6531" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6531" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6531" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6531" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6532" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6532" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6532" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6532" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6533" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6533" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6533" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6534" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6534" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6534" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6534" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6535" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6535" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6535" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6535" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6536" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6536" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6537" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6537" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6537" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6537" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6538" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6538" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6538" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6539" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6539" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6539" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6540" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6540" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6540" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6540" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6541" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6541" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6541" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6541" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6542" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6542" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6542" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6543" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6543" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6543" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6544" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6544" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6544" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6545" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6545" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6545" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6546" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6546" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6546" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6546" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6547" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6547" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6547" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6547" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6548" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6548" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6548" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6549" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6549" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6549" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6549" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6550" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6550" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6550" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6550" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6551" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6551" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6551" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6552" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6552" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6552" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6552" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6553" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6553" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6553" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6553" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6554" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6554" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6554" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6554" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6555" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6555" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6555" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6555" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6556" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6556" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6556" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6557" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6557" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6557" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6558" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6558" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6558" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6559" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6559" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6559" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6560" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6560" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6560" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6561" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6561" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6561" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6562" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6562" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6562" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6563" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6563" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6563" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6564" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6564" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6564" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6565" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6565" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6565" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6566" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6566" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6566" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6567" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6567" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6567" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6568" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6568" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6568" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6569" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6569" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6569" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6570" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6570" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6570" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6571" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6571" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6571" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6572" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6572" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6572" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6573" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6573" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6573" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6574" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6574" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6574" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6575" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6575" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6575" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6576" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6576" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6576" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6577" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6577" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6577" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6577" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6578" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6578" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6578" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6579" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6579" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6579" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6579" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6580" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6580" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6580" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6580" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6581" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6581" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6581" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6582" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6582" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6582" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6582" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6583" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6583" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6583" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6583" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6584" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6584" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6584" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6584" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6585" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6585" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6585" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6585" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6586" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6586" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6586" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6586" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6587" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6587" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6587" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6588" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6588" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6588" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6588" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6589" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6589" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6589" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6589" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6590" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6590" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6590" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6590" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6591" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6591" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6591" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6591" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6592" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6592" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6592" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6592" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6593" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6593" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6593" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6593" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6594" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6594" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6594" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6594" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6595" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6595" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6595" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6595" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6596" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6596" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6596" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6596" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6597" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6597" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6597" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6597" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6598" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6598" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6598" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6598" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6599" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6599" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6599" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6599" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6600" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6600" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6600" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6600" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6601" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6601" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6601" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6601" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6602" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6602" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6602" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6602" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6603" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6603" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6603" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6603" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6604" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6604" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6604" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6604" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6605" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6605" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6605" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6605" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6606" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6606" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6606" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6607" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6607" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6607" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6607" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6608" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6608" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6608" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6608" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6609" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6609" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6609" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6609" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6610" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6610" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6610" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6610" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6611" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6611" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6611" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6611" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6612" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6612" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6612" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6612" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6613" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6613" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6613" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6613" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6614" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6614" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6614" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6614" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6615" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6615" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6615" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6615" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6616" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6616" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6616" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6617" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6617" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6617" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6617" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6618" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6618" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6618" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6618" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6619" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6619" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6619" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6620" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6620" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6620" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6620" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6621" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6621" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6621" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6621" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6622" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6622" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6622" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6622" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6623" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6623" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6623" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6624" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6624" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6624" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6625" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6625" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6626" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6626" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6626" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6627" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6627" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6627" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6628" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6628" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6629" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6629" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6629" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6630" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6630" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6630" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6631" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6631" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6631" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6632" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6632" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6632" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6633" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6633" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6633" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6633" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6634" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6634" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6634" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6634" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6635" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6635" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6635" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6635" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6636" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6636" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6636" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6636" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6637" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6637" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6637" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6637" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6638" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6638" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6638" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6638" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6639" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6639" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6639" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6639" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6640" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6640" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6640" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6640" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6641" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6641" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6641" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6641" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6642" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6642" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6642" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6642" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6643" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6643" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6643" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6643" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6644" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6644" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6644" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6644" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6645" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6645" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6645" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6645" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6646" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6646" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6646" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6646" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6647" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6647" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6647" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6647" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6648" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6648" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6648" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6648" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6649" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6649" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6649" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6649" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6650" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6650" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6650" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6650" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6651" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6651" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6651" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6651" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6652" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6652" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6652" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6652" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6653" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6653" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6653" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6654" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6654" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6654" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6654" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6655" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6655" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6655" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6655" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6656" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6656" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6656" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6656" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6657" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6657" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6657" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6657" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6658" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6658" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6658" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6659" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6659" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6659" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6659" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6660" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6660" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6660" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6660" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6661" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6661" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6661" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6661" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6662" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6662" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6662" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6662" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6663" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6663" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6663" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6663" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6664" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6664" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6664" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6664" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6665" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6665" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6665" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6665" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6666" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6666" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6666" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6666" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6667" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6667" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6667" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6667" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6668" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6668" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6668" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6668" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6669" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6669" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6669" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6669" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6670" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6670" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6670" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6670" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6671" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6671" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6671" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6671" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6672" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6672" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6672" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6672" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6673" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6673" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6673" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6673" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6674" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6674" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6674" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6674" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6675" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6675" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6675" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6675" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6676" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6676" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6676" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6677" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6677" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6677" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6677" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6678" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6678" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6678" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6678" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6679" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6679" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6679" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6679" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6680" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6680" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6680" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6680" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6681" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6681" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6681" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6681" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6682" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6682" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6682" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6682" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6683" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6683" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6683" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6683" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6684" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6684" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6684" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6684" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6685" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6685" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6685" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6685" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6686" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6686" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6686" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6686" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6687" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6687" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6687" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6687" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6688" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6688" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6688" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6688" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6689" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6689" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6689" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6689" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6690" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6690" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6690" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6690" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6691" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6691" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6691" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6691" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6692" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6692" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6692" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6693" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6693" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6693" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6693" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6694" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6694" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6694" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6695" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6695" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6695" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6695" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6696" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6696" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6696" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6696" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6697" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6697" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6697" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6697" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6698" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6698" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6698" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6698" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6699" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6699" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6699" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6699" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6700" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6700" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6700" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6700" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6701" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6701" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6701" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6701" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6702" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6702" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6702" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6702" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6703" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6703" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6703" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6703" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6704" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6704" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6704" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6704" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6705" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6705" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6705" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6705" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6706" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6706" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6706" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6706" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6707" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6707" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6707" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6707" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6708" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6708" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6708" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6708" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6709" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6709" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6709" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6709" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6710" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6710" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6710" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6710" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6711" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6711" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6711" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6711" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6712" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6712" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6712" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6712" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6713" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6713" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6713" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6713" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6714" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6714" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6714" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6714" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6715" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6715" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6715" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6715" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6716" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6716" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6716" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6716" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6717" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6717" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6717" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6717" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6718" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6718" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6718" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6718" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6719" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6719" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6719" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6719" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C6351"/>
+  <autoFilter ref="A1:C6719"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>